<commit_message>
Single Pricipal Responsibility Pattern
</commit_message>
<xml_diff>
--- a/resources/testData/testdata.xlsx
+++ b/resources/testData/testdata.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>10:45 AM</t>
   </si>
@@ -78,25 +78,22 @@
     <t>Cypress.docx</t>
   </si>
   <si>
-    <t>Test21</t>
-  </si>
-  <si>
-    <t>Test22</t>
-  </si>
-  <si>
-    <t>29</t>
-  </si>
-  <si>
-    <t>Sanity23</t>
-  </si>
-  <si>
-    <t>Sanity24</t>
-  </si>
-  <si>
-    <t>Sanity23.Test23@gmail.com</t>
-  </si>
-  <si>
-    <t>Sanity24.Test24@gmail.com</t>
+    <t>Sanity31</t>
+  </si>
+  <si>
+    <t>Sanity32</t>
+  </si>
+  <si>
+    <t>Test31</t>
+  </si>
+  <si>
+    <t>Test32</t>
+  </si>
+  <si>
+    <t>Sanity31.Test31@gmail.com</t>
+  </si>
+  <si>
+    <t>Sanity32.Test32@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -459,7 +456,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="A1:XFD1048576"/>
+      <selection activeCell="G3" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -509,25 +506,25 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>0</v>
@@ -541,16 +538,16 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E3" s="6" t="s">
         <v>13</v>

</xml_diff>